<commit_message>
Mean ROC curve done using bootstrap.
</commit_message>
<xml_diff>
--- a/PaperNeural/ResultsControl Bkp/ResultsControlFinal.xlsx
+++ b/PaperNeural/ResultsControl Bkp/ResultsControlFinal.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="3800" yWindow="1140" windowWidth="25600" windowHeight="18540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Detail" sheetId="2" r:id="rId2"/>
+    <sheet name="GrandConfusion" sheetId="3" r:id="rId3"/>
+    <sheet name="TP_GM_stats" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Overview!$A$1:$O$1</definedName>
@@ -30,8 +32,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Fábio Henrique Monteiro Oliveira</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Fábio Henrique Monteiro Oliveira:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+True positive general mean of all tasks and all datasets.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="183">
   <si>
     <t>ID</t>
   </si>
@@ -533,12 +567,141 @@
   <si>
     <t>ResultsMar2017-t-SNE_MI_5000_LR_700_PE_50.xlsx</t>
   </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>H</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PD</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DBS</t>
+    </r>
+  </si>
+  <si>
+    <t>Cross-Validation</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Target Class</t>
+  </si>
+  <si>
+    <t>Output Class</t>
+  </si>
+  <si>
+    <t>PCA</t>
+  </si>
+  <si>
+    <t>Sammons</t>
+  </si>
+  <si>
+    <t>t-SNE (perp 17-51)</t>
+  </si>
+  <si>
+    <t>The Wilcoxon rank sum test is equivalent to the Mann-Whitney U-test.</t>
+  </si>
+  <si>
+    <t>t-SNE</t>
+  </si>
+  <si>
+    <t>P-Value</t>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>H</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PD</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DBS</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -570,16 +733,99 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -587,19 +833,191 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -877,12 +1295,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O152"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8052,6 +8470,7 @@
   <autoFilter ref="A1:O1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -41904,4 +42323,1279 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:M25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="22"/>
+      <c r="H2" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="22"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="4"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="4"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" s="24">
+        <v>0.59999999999999987</v>
+      </c>
+      <c r="D6" s="3">
+        <v>7.5892857142857137E-2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.10119047619047618</v>
+      </c>
+      <c r="F6" s="4">
+        <v>77.211796246648802</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="J6" s="24">
+        <v>0.70238095238095233</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.11210317460317462</v>
+      </c>
+      <c r="L6" s="3">
+        <v>7.4735449735449752E-2</v>
+      </c>
+      <c r="M6" s="4">
+        <v>78.988471550762355</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A7" s="19"/>
+      <c r="B7" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.31428571428571433</v>
+      </c>
+      <c r="D7" s="24">
+        <v>0.7901785714285714</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.25595238095238093</v>
+      </c>
+      <c r="F7" s="4">
+        <v>58.083570334718878</v>
+      </c>
+      <c r="H7" s="19"/>
+      <c r="I7" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.2412698412698413</v>
+      </c>
+      <c r="K7" s="24">
+        <v>0.77579365079365081</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0.19841269841269837</v>
+      </c>
+      <c r="M7" s="4">
+        <v>63.826314071172057</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A8" s="19"/>
+      <c r="B8" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C8" s="3">
+        <v>8.5714285714285729E-2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.13392857142857142</v>
+      </c>
+      <c r="E8" s="24">
+        <v>0.6428571428571429</v>
+      </c>
+      <c r="F8" s="4">
+        <v>74.534161490683232</v>
+      </c>
+      <c r="H8" s="19"/>
+      <c r="I8" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="J8" s="3">
+        <v>5.4761904761904769E-2</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0.11210317460317462</v>
+      </c>
+      <c r="L8" s="24">
+        <v>0.72023809523809523</v>
+      </c>
+      <c r="M8" s="4">
+        <v>81.189890404831132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3">
+        <v>59.999999999999986</v>
+      </c>
+      <c r="D9" s="3">
+        <v>79.017857142857139</v>
+      </c>
+      <c r="E9" s="3">
+        <v>64.285714285714292</v>
+      </c>
+      <c r="F9" s="25">
+        <v>67.767857142857139</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3">
+        <v>70.238095238095227</v>
+      </c>
+      <c r="K9" s="3">
+        <v>77.579365079365076</v>
+      </c>
+      <c r="L9" s="3">
+        <v>72.023809523809518</v>
+      </c>
+      <c r="M9" s="25">
+        <v>73.481298081174302</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="4"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="4"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="4"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="M13" s="4"/>
+    </row>
+    <row r="14" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A14" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C14" s="24">
+        <v>0.77857142857142847</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.11124999999999996</v>
+      </c>
+      <c r="E14" s="3">
+        <v>7.9285714285714279E-2</v>
+      </c>
+      <c r="F14" s="4">
+        <v>80.339045513174867</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="J14" s="24">
+        <v>0.79492063492063492</v>
+      </c>
+      <c r="K14" s="3">
+        <v>7.6230158730158731E-2</v>
+      </c>
+      <c r="L14" s="3">
+        <v>4.9047619047619034E-2</v>
+      </c>
+      <c r="M14" s="4">
+        <v>86.38578636422443</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A15" s="19"/>
+      <c r="B15" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.16571428571428573</v>
+      </c>
+      <c r="D15" s="24">
+        <v>0.7628571428571429</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.23857142857142855</v>
+      </c>
+      <c r="F15" s="4">
+        <v>65.361077111383111</v>
+      </c>
+      <c r="H15" s="19"/>
+      <c r="I15" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0.14879365079365076</v>
+      </c>
+      <c r="K15" s="24">
+        <v>0.79101190476190464</v>
+      </c>
+      <c r="L15" s="3">
+        <v>0.18111111111111108</v>
+      </c>
+      <c r="M15" s="4">
+        <v>70.568306127000668</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A16" s="19"/>
+      <c r="B16" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C16" s="3">
+        <v>5.571428571428573E-2</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.12589285714285714</v>
+      </c>
+      <c r="E16" s="24">
+        <v>0.68214285714285705</v>
+      </c>
+      <c r="F16" s="4">
+        <v>78.974571015091996</v>
+      </c>
+      <c r="H16" s="19"/>
+      <c r="I16" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="J16" s="3">
+        <v>5.3238095238095251E-2</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0.13275793650793649</v>
+      </c>
+      <c r="L16" s="24">
+        <v>0.76592592592592612</v>
+      </c>
+      <c r="M16" s="4">
+        <v>80.460999954144569</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3">
+        <v>77.857142857142847</v>
+      </c>
+      <c r="D17" s="3">
+        <v>76.285714285714292</v>
+      </c>
+      <c r="E17" s="3">
+        <v>68.214285714285708</v>
+      </c>
+      <c r="F17" s="25">
+        <v>74.119047619047606</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3">
+        <v>79.492063492063494</v>
+      </c>
+      <c r="K17" s="3">
+        <v>79.101190476190467</v>
+      </c>
+      <c r="L17" s="3">
+        <v>76.592592592592609</v>
+      </c>
+      <c r="M17" s="25">
+        <v>78.57765996563451</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="4"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="4"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="4"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="4"/>
+    </row>
+    <row r="20" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="4"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="J20" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="4"/>
+    </row>
+    <row r="21" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="M21" s="4"/>
+    </row>
+    <row r="22" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A22" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C22" s="24">
+        <v>0.7717142857142858</v>
+      </c>
+      <c r="D22" s="3">
+        <v>8.0476190476190479E-2</v>
+      </c>
+      <c r="E22" s="3">
+        <v>7.1031746031746043E-2</v>
+      </c>
+      <c r="F22" s="4">
+        <v>83.589223389440022</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="J22" s="24">
+        <v>0.97616931216931235</v>
+      </c>
+      <c r="K22" s="3">
+        <v>1.0343915343915338E-2</v>
+      </c>
+      <c r="L22" s="3">
+        <v>1.033509700176367E-2</v>
+      </c>
+      <c r="M22" s="4">
+        <v>97.925560806280103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A23" s="19"/>
+      <c r="B23" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.13704761904761914</v>
+      </c>
+      <c r="D23" s="24">
+        <v>0.78386904761904763</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.18500000000000005</v>
+      </c>
+      <c r="F23" s="4">
+        <v>70.87957630493986</v>
+      </c>
+      <c r="H23" s="19"/>
+      <c r="I23" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="J23" s="3">
+        <v>1.5259259259259255E-2</v>
+      </c>
+      <c r="K23" s="24">
+        <v>0.97532407407407407</v>
+      </c>
+      <c r="L23" s="3">
+        <v>3.493827160493828E-2</v>
+      </c>
+      <c r="M23" s="4">
+        <v>95.105170810397595</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A24" s="19"/>
+      <c r="B24" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C24" s="3">
+        <v>9.123809523809516E-2</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.13565476190476186</v>
+      </c>
+      <c r="E24" s="24">
+        <v>0.74396825396825383</v>
+      </c>
+      <c r="F24" s="4">
+        <v>76.629730602435245</v>
+      </c>
+      <c r="H24" s="19"/>
+      <c r="I24" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="J24" s="3">
+        <v>8.5185185185185173E-3</v>
+      </c>
+      <c r="K24" s="3">
+        <v>1.4332010582010583E-2</v>
+      </c>
+      <c r="L24" s="24">
+        <v>0.95412698412698393</v>
+      </c>
+      <c r="M24" s="4">
+        <v>97.661099790819051</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9">
+        <v>77.171428571428578</v>
+      </c>
+      <c r="D25" s="9">
+        <v>78.386904761904759</v>
+      </c>
+      <c r="E25" s="9">
+        <v>74.396825396825378</v>
+      </c>
+      <c r="F25" s="27">
+        <v>76.651719576719572</v>
+      </c>
+      <c r="H25" s="8"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9">
+        <v>97.616931216931235</v>
+      </c>
+      <c r="K25" s="9">
+        <v>97.532407407407405</v>
+      </c>
+      <c r="L25" s="9">
+        <v>95.41269841269839</v>
+      </c>
+      <c r="M25" s="29">
+        <v>96.875084527498629</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="H22:H24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M27"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="22"/>
+      <c r="H3" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="22"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="4"/>
+      <c r="H5" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="M6" s="4"/>
+    </row>
+    <row r="7" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A7" s="19"/>
+      <c r="B7" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.10911304082262396</v>
+      </c>
+      <c r="E7" s="6">
+        <v>9.1357667628379963E-2</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="J7" s="12">
+        <v>1</v>
+      </c>
+      <c r="K7" s="12">
+        <v>0.10941653896157671</v>
+      </c>
+      <c r="L7" s="12">
+        <v>9.1162428852920183E-2</v>
+      </c>
+      <c r="M7" s="7"/>
+    </row>
+    <row r="8" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A8" s="19"/>
+      <c r="B8" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.10911304082262396</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1</v>
+      </c>
+      <c r="E8" s="15">
+        <v>8.5087875182818658E-14</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="J8" s="12">
+        <v>0.10941653896157671</v>
+      </c>
+      <c r="K8" s="12">
+        <v>1</v>
+      </c>
+      <c r="L8" s="12">
+        <v>0.22117846301415736</v>
+      </c>
+      <c r="M8" s="7"/>
+    </row>
+    <row r="9" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A9" s="19"/>
+      <c r="B9" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C9" s="6">
+        <v>9.1357667628379963E-2</v>
+      </c>
+      <c r="D9" s="15">
+        <v>8.5087875182818658E-14</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="J9" s="12">
+        <v>9.1162428852920183E-2</v>
+      </c>
+      <c r="K9" s="12">
+        <v>0.22117846301415736</v>
+      </c>
+      <c r="L9" s="12">
+        <v>1</v>
+      </c>
+      <c r="M9" s="7"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="7"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="7"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="4"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="4"/>
+      <c r="H13" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="I13" s="5"/>
+      <c r="J13" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="4"/>
+    </row>
+    <row r="14" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="M14" s="4"/>
+    </row>
+    <row r="15" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="19"/>
+      <c r="B15" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0.10947722499234211</v>
+      </c>
+      <c r="E15" s="6">
+        <v>9.1506303541128917E-2</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="J15" s="12">
+        <v>1</v>
+      </c>
+      <c r="K15" s="12">
+        <v>0.25585172369068165</v>
+      </c>
+      <c r="L15" s="12">
+        <v>0.85512330350816912</v>
+      </c>
+      <c r="M15" s="7"/>
+    </row>
+    <row r="16" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A16" s="19"/>
+      <c r="B16" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0.10947722499234211</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1</v>
+      </c>
+      <c r="E16" s="15">
+        <v>8.6150724896200906E-14</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="J16" s="12">
+        <v>0.25585172369068165</v>
+      </c>
+      <c r="K16" s="12">
+        <v>1</v>
+      </c>
+      <c r="L16" s="16">
+        <v>3.3180763002265924E-3</v>
+      </c>
+      <c r="M16" s="7"/>
+    </row>
+    <row r="17" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A17" s="19"/>
+      <c r="B17" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C17" s="6">
+        <v>9.1506303541128917E-2</v>
+      </c>
+      <c r="D17" s="15">
+        <v>8.6150724896200906E-14</v>
+      </c>
+      <c r="E17" s="6">
+        <v>1</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="J17" s="12">
+        <v>0.85512330350816912</v>
+      </c>
+      <c r="K17" s="16">
+        <v>3.3180763002265924E-3</v>
+      </c>
+      <c r="L17" s="12">
+        <v>1</v>
+      </c>
+      <c r="M17" s="7"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="7"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="7"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="4"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="4"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="4"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="4"/>
+    </row>
+    <row r="21" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="4"/>
+      <c r="H21" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="I21" s="5"/>
+      <c r="J21" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="4"/>
+    </row>
+    <row r="22" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="M22" s="4"/>
+    </row>
+    <row r="23" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A23" s="19"/>
+      <c r="B23" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C23" s="6">
+        <v>1</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.10929515328132222</v>
+      </c>
+      <c r="E23" s="6">
+        <v>9.1299985261016986E-2</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="J23" s="12">
+        <v>1</v>
+      </c>
+      <c r="K23" s="12">
+        <v>0.25577002714792502</v>
+      </c>
+      <c r="L23" s="12">
+        <v>0.10048333285904035</v>
+      </c>
+      <c r="M23" s="7"/>
+    </row>
+    <row r="24" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A24" s="19"/>
+      <c r="B24" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0.10929515328132222</v>
+      </c>
+      <c r="D24" s="6">
+        <v>1</v>
+      </c>
+      <c r="E24" s="15">
+        <v>8.4755539325322942E-14</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="J24" s="12">
+        <v>0.25577002714792502</v>
+      </c>
+      <c r="K24" s="12">
+        <v>1</v>
+      </c>
+      <c r="L24" s="16">
+        <v>1.5530595855300269E-8</v>
+      </c>
+      <c r="M24" s="7"/>
+    </row>
+    <row r="25" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A25" s="19"/>
+      <c r="B25" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C25" s="6">
+        <v>9.1299985261016986E-2</v>
+      </c>
+      <c r="D25" s="15">
+        <v>8.4755539325322942E-14</v>
+      </c>
+      <c r="E25" s="6">
+        <v>1</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="J25" s="12">
+        <v>0.10048333285904035</v>
+      </c>
+      <c r="K25" s="16">
+        <v>1.5530595855300269E-8</v>
+      </c>
+      <c r="L25" s="12">
+        <v>1</v>
+      </c>
+      <c r="M25" s="7"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="11"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="7"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="8"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="10"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="H3:M3"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="H7:H9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>